<commit_message>
dynamo script and xlsx with distances added
</commit_message>
<xml_diff>
--- a/coords_test_polygon.xlsx
+++ b/coords_test_polygon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\000_Buro_Happold\EmLi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B2BF61-243A-4016-8DEF-BD3BE09EDB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE16499-312B-4846-938D-4F1E69EF1732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7616EF13-6BBA-43AA-9732-4F1E79D84DA4}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W23" sqref="W23"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,18 +411,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -443,10 +443,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>